<commit_message>
Update rank [2026-01-28 04:04]
</commit_message>
<xml_diff>
--- a/플레이스_순위_통합기록.xlsx
+++ b/플레이스_순위_통합기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,6 +463,19 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-01-28 04:01</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>39</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update rank 2026-01-28 04:08
</commit_message>
<xml_diff>
--- a/플레이스_순위_통합기록.xlsx
+++ b/플레이스_순위_통합기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,19 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-01-28 04:05</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>39</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update rank 2026-01-28 04:38
</commit_message>
<xml_diff>
--- a/플레이스_순위_통합기록.xlsx
+++ b/플레이스_순위_통합기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,19 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-01-28 04:35</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update rank 2026-01-28 10:02
</commit_message>
<xml_diff>
--- a/플레이스_순위_통합기록.xlsx
+++ b/플레이스_순위_통합기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,6 +502,19 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:59</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>39</v>
+      </c>
+      <c r="C6" t="n">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update rank 2026-01-29 05:18
</commit_message>
<xml_diff>
--- a/플레이스_순위_통합기록.xlsx
+++ b/플레이스_순위_통합기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,6 +515,19 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-01-29 05:15</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>33</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update rank 2026-01-29 11:07
</commit_message>
<xml_diff>
--- a/플레이스_순위_통합기록.xlsx
+++ b/플레이스_순위_통합기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,6 +528,19 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-01-29 11:04</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>33</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update rank 2026-01-30 05:36
</commit_message>
<xml_diff>
--- a/플레이스_순위_통합기록.xlsx
+++ b/플레이스_순위_통합기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,6 +541,19 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-01-30 05:34</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>36</v>
+      </c>
+      <c r="C9" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update rank 2026-01-30 10:09
</commit_message>
<xml_diff>
--- a/플레이스_순위_통합기록.xlsx
+++ b/플레이스_순위_통합기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,19 @@
         <v>6</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-01-30 10:06</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>36</v>
+      </c>
+      <c r="C10" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update rank 2026-01-31 05:13
</commit_message>
<xml_diff>
--- a/플레이스_순위_통합기록.xlsx
+++ b/플레이스_순위_통합기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,6 +567,19 @@
         <v>6</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-01-31 05:10</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>23</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update rank 2026-01-31 10:11
</commit_message>
<xml_diff>
--- a/플레이스_순위_통합기록.xlsx
+++ b/플레이스_순위_통합기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -580,6 +580,19 @@
         <v>5</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-01-31 10:08</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>23</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>